<commit_message>
new resources into the game
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed100b9df88b388/Documents/GitHub/Fishing-Pomodoro-Timer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDBB80E8-B8CE-484C-A9C6-39D46A863886}"/>
+  <xr:revisionPtr revIDLastSave="466" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98F0484B-6D7C-4BE6-85FD-A6713C72578D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
+    <workbookView xWindow="-19310" yWindow="-1350" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
   </bookViews>
   <sheets>
     <sheet name="catchables" sheetId="1" r:id="rId1"/>
@@ -1039,9 +1039,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>183480</xdr:colOff>
+      <xdr:colOff>186655</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>47095</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1106,7 +1106,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>442440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>107935</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1549,7 +1549,7 @@
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView zoomScale="116" zoomScaleNormal="350" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1598,8 +1598,8 @@
         <v>240</v>
       </c>
       <c r="F2">
-        <f ca="1">ROUND(RAND()*((C2 * 10)-(C2*5))+ C2*5,0)</f>
-        <v>28</v>
+        <f t="shared" ref="F2:F33" ca="1" si="0">ROUND(RAND()*((C2 * 10)-(C2*5))+ C2*5,0)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1619,8 +1619,8 @@
         <v>240</v>
       </c>
       <c r="F3">
-        <f ca="1">ROUND(RAND()*((C3 * 10)-(C3*5))+ C3*5,0)</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1640,8 +1640,8 @@
         <v>240</v>
       </c>
       <c r="F4">
-        <f ca="1">ROUND(RAND()*((C4 * 10)-(C4*5))+ C4*5,0)</f>
-        <v>78</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1661,8 +1661,8 @@
         <v>240</v>
       </c>
       <c r="F5">
-        <f ca="1">ROUND(RAND()*((C5 * 10)-(C5*5))+ C5*5,0)</f>
-        <v>68</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1682,8 +1682,8 @@
         <v>240</v>
       </c>
       <c r="F6">
-        <f ca="1">ROUND(RAND()*((C6 * 10)-(C6*5))+ C6*5,0)</f>
-        <v>52</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,8 +1703,8 @@
         <v>240</v>
       </c>
       <c r="F7">
-        <f ca="1">ROUND(RAND()*((C7 * 10)-(C7*5))+ C7*5,0)</f>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1724,8 +1724,8 @@
         <v>240</v>
       </c>
       <c r="F8">
-        <f ca="1">ROUND(RAND()*((C8 * 10)-(C8*5))+ C8*5,0)</f>
-        <v>123</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1745,8 +1745,8 @@
         <v>240</v>
       </c>
       <c r="F9">
-        <f ca="1">ROUND(RAND()*((C9 * 10)-(C9*5))+ C9*5,0)</f>
-        <v>129</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1766,8 +1766,8 @@
         <v>240</v>
       </c>
       <c r="F10">
-        <f ca="1">ROUND(RAND()*((C10 * 10)-(C10*5))+ C10*5,0)</f>
-        <v>13</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1787,8 +1787,8 @@
         <v>251</v>
       </c>
       <c r="F11">
-        <f ca="1">ROUND(RAND()*((C11 * 10)-(C11*5))+ C11*5,0)</f>
-        <v>28</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,8 +1808,8 @@
         <v>251</v>
       </c>
       <c r="F12">
-        <f ca="1">ROUND(RAND()*((C12 * 10)-(C12*5))+ C12*5,0)</f>
-        <v>63</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1829,8 +1829,8 @@
         <v>251</v>
       </c>
       <c r="F13">
-        <f ca="1">ROUND(RAND()*((C13 * 10)-(C13*5))+ C13*5,0)</f>
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1850,8 +1850,8 @@
         <v>240</v>
       </c>
       <c r="F14">
-        <f ca="1">ROUND(RAND()*((C14 * 10)-(C14*5))+ C14*5,0)</f>
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1871,8 +1871,8 @@
         <v>256</v>
       </c>
       <c r="F15">
-        <f ca="1">ROUND(RAND()*((C15 * 10)-(C15*5))+ C15*5,0)</f>
-        <v>150</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,8 +1892,8 @@
         <v>256</v>
       </c>
       <c r="F16">
-        <f ca="1">ROUND(RAND()*((C16 * 10)-(C16*5))+ C16*5,0)</f>
-        <v>158</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,8 +1913,8 @@
         <v>259</v>
       </c>
       <c r="F17">
-        <f ca="1">ROUND(RAND()*((C17 * 10)-(C17*5))+ C17*5,0)</f>
-        <v>118</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,8 +1934,8 @@
         <v>240</v>
       </c>
       <c r="F18">
-        <f ca="1">ROUND(RAND()*((C18 * 10)-(C18*5))+ C18*5,0)</f>
-        <v>59</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1955,8 +1955,8 @@
         <v>253</v>
       </c>
       <c r="F19">
-        <f ca="1">ROUND(RAND()*((C19 * 10)-(C19*5))+ C19*5,0)</f>
-        <v>67</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,8 +1976,8 @@
         <v>252</v>
       </c>
       <c r="F20">
-        <f ca="1">ROUND(RAND()*((C20 * 10)-(C20*5))+ C20*5,0)</f>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,8 +1997,8 @@
         <v>253</v>
       </c>
       <c r="F21">
-        <f ca="1">ROUND(RAND()*((C21 * 10)-(C21*5))+ C21*5,0)</f>
-        <v>86</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,8 +2018,8 @@
         <v>253</v>
       </c>
       <c r="F22">
-        <f ca="1">ROUND(RAND()*((C22 * 10)-(C22*5))+ C22*5,0)</f>
-        <v>52</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
         <v>256</v>
       </c>
       <c r="F23">
-        <f ca="1">ROUND(RAND()*((C23 * 10)-(C23*5))+ C23*5,0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
     </row>
@@ -2060,8 +2060,8 @@
         <v>251</v>
       </c>
       <c r="F24">
-        <f ca="1">ROUND(RAND()*((C24 * 10)-(C24*5))+ C24*5,0)</f>
-        <v>26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2081,8 +2081,8 @@
         <v>251</v>
       </c>
       <c r="F25">
-        <f ca="1">ROUND(RAND()*((C25 * 10)-(C25*5))+ C25*5,0)</f>
-        <v>72</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2102,8 +2102,8 @@
         <v>251</v>
       </c>
       <c r="F26">
-        <f ca="1">ROUND(RAND()*((C26 * 10)-(C26*5))+ C26*5,0)</f>
-        <v>45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2123,8 +2123,8 @@
         <v>254</v>
       </c>
       <c r="F27">
-        <f ca="1">ROUND(RAND()*((C27 * 10)-(C27*5))+ C27*5,0)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,8 +2144,8 @@
         <v>254</v>
       </c>
       <c r="F28">
-        <f ca="1">ROUND(RAND()*((C28 * 10)-(C28*5))+ C28*5,0)</f>
-        <v>68</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2165,8 +2165,8 @@
         <v>254</v>
       </c>
       <c r="F29">
-        <f ca="1">ROUND(RAND()*((C29 * 10)-(C29*5))+ C29*5,0)</f>
-        <v>61</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2186,8 +2186,8 @@
         <v>254</v>
       </c>
       <c r="F30">
-        <f ca="1">ROUND(RAND()*((C30 * 10)-(C30*5))+ C30*5,0)</f>
-        <v>85</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,8 +2207,8 @@
         <v>255</v>
       </c>
       <c r="F31">
-        <f ca="1">ROUND(RAND()*((C31 * 10)-(C31*5))+ C31*5,0)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,8 +2228,8 @@
         <v>255</v>
       </c>
       <c r="F32">
-        <f ca="1">ROUND(RAND()*((C32 * 10)-(C32*5))+ C32*5,0)</f>
-        <v>76</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2249,8 +2249,8 @@
         <v>255</v>
       </c>
       <c r="F33">
-        <f ca="1">ROUND(RAND()*((C33 * 10)-(C33*5))+ C33*5,0)</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2270,8 +2270,8 @@
         <v>254</v>
       </c>
       <c r="F34">
-        <f ca="1">ROUND(RAND()*((C34 * 10)-(C34*5))+ C34*5,0)</f>
-        <v>59</v>
+        <f t="shared" ref="F34:F65" ca="1" si="1">ROUND(RAND()*((C34 * 10)-(C34*5))+ C34*5,0)</f>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2291,8 +2291,8 @@
         <v>254</v>
       </c>
       <c r="F35">
-        <f ca="1">ROUND(RAND()*((C35 * 10)-(C35*5))+ C35*5,0)</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2312,8 +2312,8 @@
         <v>256</v>
       </c>
       <c r="F36">
-        <f ca="1">ROUND(RAND()*((C36 * 10)-(C36*5))+ C36*5,0)</f>
-        <v>44</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,8 +2333,8 @@
         <v>253</v>
       </c>
       <c r="F37">
-        <f ca="1">ROUND(RAND()*((C37 * 10)-(C37*5))+ C37*5,0)</f>
-        <v>22</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2354,8 +2354,8 @@
         <v>257</v>
       </c>
       <c r="F38">
-        <f ca="1">ROUND(RAND()*((C38 * 10)-(C38*5))+ C38*5,0)</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>257</v>
       </c>
       <c r="F39">
-        <f ca="1">ROUND(RAND()*((C39 * 10)-(C39*5))+ C39*5,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>89</v>
       </c>
     </row>
@@ -2396,8 +2396,8 @@
         <v>256</v>
       </c>
       <c r="F40">
-        <f ca="1">ROUND(RAND()*((C40 * 10)-(C40*5))+ C40*5,0)</f>
-        <v>115</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2417,8 +2417,8 @@
         <v>257</v>
       </c>
       <c r="F41">
-        <f ca="1">ROUND(RAND()*((C41 * 10)-(C41*5))+ C41*5,0)</f>
-        <v>54</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2438,8 +2438,8 @@
         <v>251</v>
       </c>
       <c r="F42">
-        <f ca="1">ROUND(RAND()*((C42 * 10)-(C42*5))+ C42*5,0)</f>
-        <v>65</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2459,8 +2459,8 @@
         <v>259</v>
       </c>
       <c r="F43">
-        <f ca="1">ROUND(RAND()*((C43 * 10)-(C43*5))+ C43*5,0)</f>
-        <v>50</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2480,8 +2480,8 @@
         <v>254</v>
       </c>
       <c r="F44">
-        <f ca="1">ROUND(RAND()*((C44 * 10)-(C44*5))+ C44*5,0)</f>
-        <v>96</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2501,8 +2501,8 @@
         <v>259</v>
       </c>
       <c r="F45">
-        <f ca="1">ROUND(RAND()*((C45 * 10)-(C45*5))+ C45*5,0)</f>
-        <v>109</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,8 +2522,8 @@
         <v>253</v>
       </c>
       <c r="F46">
-        <f ca="1">ROUND(RAND()*((C46 * 10)-(C46*5))+ C46*5,0)</f>
-        <v>43</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2543,8 +2543,8 @@
         <v>253</v>
       </c>
       <c r="F47">
-        <f ca="1">ROUND(RAND()*((C47 * 10)-(C47*5))+ C47*5,0)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2564,8 +2564,8 @@
         <v>259</v>
       </c>
       <c r="F48">
-        <f ca="1">ROUND(RAND()*((C48 * 10)-(C48*5))+ C48*5,0)</f>
-        <v>31</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2585,8 +2585,8 @@
         <v>259</v>
       </c>
       <c r="F49">
-        <f ca="1">ROUND(RAND()*((C49 * 10)-(C49*5))+ C49*5,0)</f>
-        <v>53</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2606,8 +2606,8 @@
         <v>256</v>
       </c>
       <c r="F50">
-        <f ca="1">ROUND(RAND()*((C50 * 10)-(C50*5))+ C50*5,0)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2627,8 +2627,8 @@
         <v>256</v>
       </c>
       <c r="F51">
-        <f ca="1">ROUND(RAND()*((C51 * 10)-(C51*5))+ C51*5,0)</f>
-        <v>83</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2648,8 +2648,8 @@
         <v>259</v>
       </c>
       <c r="F52">
-        <f ca="1">ROUND(RAND()*((C52 * 10)-(C52*5))+ C52*5,0)</f>
-        <v>123</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,8 +2669,8 @@
         <v>240</v>
       </c>
       <c r="F53">
-        <f ca="1">ROUND(RAND()*((C53 * 10)-(C53*5))+ C53*5,0)</f>
-        <v>52</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2690,8 +2690,8 @@
         <v>259</v>
       </c>
       <c r="F54">
-        <f ca="1">ROUND(RAND()*((C54 * 10)-(C54*5))+ C54*5,0)</f>
-        <v>70</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2711,8 +2711,8 @@
         <v>259</v>
       </c>
       <c r="F55">
-        <f ca="1">ROUND(RAND()*((C55 * 10)-(C55*5))+ C55*5,0)</f>
-        <v>62</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2732,8 +2732,8 @@
         <v>251</v>
       </c>
       <c r="F56">
-        <f ca="1">ROUND(RAND()*((C56 * 10)-(C56*5))+ C56*5,0)</f>
-        <v>56</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2753,8 +2753,8 @@
         <v>257</v>
       </c>
       <c r="F57">
-        <f ca="1">ROUND(RAND()*((C57 * 10)-(C57*5))+ C57*5,0)</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2774,8 +2774,8 @@
         <v>256</v>
       </c>
       <c r="F58">
-        <f ca="1">ROUND(RAND()*((C58 * 10)-(C58*5))+ C58*5,0)</f>
-        <v>149</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,8 +2795,8 @@
         <v>256</v>
       </c>
       <c r="F59">
-        <f ca="1">ROUND(RAND()*((C59 * 10)-(C59*5))+ C59*5,0)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2816,8 +2816,8 @@
         <v>256</v>
       </c>
       <c r="F60">
-        <f ca="1">ROUND(RAND()*((C60 * 10)-(C60*5))+ C60*5,0)</f>
-        <v>79</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2837,8 +2837,8 @@
         <v>245</v>
       </c>
       <c r="F61">
-        <f ca="1">ROUND(RAND()*((C61 * 10)-(C61*5))+ C61*5,0)</f>
-        <v>114</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2858,8 +2858,8 @@
         <v>244</v>
       </c>
       <c r="F62">
-        <f ca="1">ROUND(RAND()*((C62 * 10)-(C62*5))+ C62*5,0)</f>
-        <v>79</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2879,8 +2879,8 @@
         <v>244</v>
       </c>
       <c r="F63">
-        <f ca="1">ROUND(RAND()*((C63 * 10)-(C63*5))+ C63*5,0)</f>
-        <v>90</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>244</v>
       </c>
       <c r="F64">
-        <f ca="1">ROUND(RAND()*((C64 * 10)-(C64*5))+ C64*5,0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>158</v>
       </c>
     </row>
@@ -2921,8 +2921,8 @@
         <v>244</v>
       </c>
       <c r="F65">
-        <f ca="1">ROUND(RAND()*((C65 * 10)-(C65*5))+ C65*5,0)</f>
-        <v>128</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2942,8 +2942,8 @@
         <v>244</v>
       </c>
       <c r="F66">
-        <f ca="1">ROUND(RAND()*((C66 * 10)-(C66*5))+ C66*5,0)</f>
-        <v>75</v>
+        <f t="shared" ref="F66:F97" ca="1" si="2">ROUND(RAND()*((C66 * 10)-(C66*5))+ C66*5,0)</f>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2963,8 +2963,8 @@
         <v>252</v>
       </c>
       <c r="F67">
-        <f ca="1">ROUND(RAND()*((C67 * 10)-(C67*5))+ C67*5,0)</f>
-        <v>53</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2984,8 +2984,8 @@
         <v>253</v>
       </c>
       <c r="F68">
-        <f ca="1">ROUND(RAND()*((C68 * 10)-(C68*5))+ C68*5,0)</f>
-        <v>45</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3005,8 +3005,8 @@
         <v>253</v>
       </c>
       <c r="F69">
-        <f ca="1">ROUND(RAND()*((C69 * 10)-(C69*5))+ C69*5,0)</f>
-        <v>104</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3026,8 +3026,8 @@
         <v>254</v>
       </c>
       <c r="F70">
-        <f ca="1">ROUND(RAND()*((C70 * 10)-(C70*5))+ C70*5,0)</f>
-        <v>55</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3047,8 +3047,8 @@
         <v>259</v>
       </c>
       <c r="F71">
-        <f ca="1">ROUND(RAND()*((C71 * 10)-(C71*5))+ C71*5,0)</f>
-        <v>43</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3068,8 +3068,8 @@
         <v>259</v>
       </c>
       <c r="F72">
-        <f ca="1">ROUND(RAND()*((C72 * 10)-(C72*5))+ C72*5,0)</f>
-        <v>37</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,8 +3089,8 @@
         <v>251</v>
       </c>
       <c r="F73">
-        <f ca="1">ROUND(RAND()*((C73 * 10)-(C73*5))+ C73*5,0)</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3110,8 +3110,8 @@
         <v>295</v>
       </c>
       <c r="F74">
-        <f ca="1">ROUND(RAND()*((C74 * 10)-(C74*5))+ C74*5,0)</f>
-        <v>39</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3131,8 +3131,8 @@
         <v>253</v>
       </c>
       <c r="F75">
-        <f ca="1">ROUND(RAND()*((C75 * 10)-(C75*5))+ C75*5,0)</f>
-        <v>59</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3152,8 +3152,8 @@
         <v>258</v>
       </c>
       <c r="F76">
-        <f ca="1">ROUND(RAND()*((C76 * 10)-(C76*5))+ C76*5,0)</f>
-        <v>68</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3173,8 +3173,8 @@
         <v>244</v>
       </c>
       <c r="F77">
-        <f ca="1">ROUND(RAND()*((C77 * 10)-(C77*5))+ C77*5,0)</f>
-        <v>64</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,8 +3194,8 @@
         <v>295</v>
       </c>
       <c r="F78">
-        <f ca="1">ROUND(RAND()*((C78 * 10)-(C78*5))+ C78*5,0)</f>
-        <v>40</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,8 +3215,8 @@
         <v>259</v>
       </c>
       <c r="F79">
-        <f ca="1">ROUND(RAND()*((C79 * 10)-(C79*5))+ C79*5,0)</f>
-        <v>23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3236,8 +3236,8 @@
         <v>255</v>
       </c>
       <c r="F80">
-        <f ca="1">ROUND(RAND()*((C80 * 10)-(C80*5))+ C80*5,0)</f>
-        <v>37</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3257,8 +3257,8 @@
         <v>255</v>
       </c>
       <c r="F81">
-        <f ca="1">ROUND(RAND()*((C81 * 10)-(C81*5))+ C81*5,0)</f>
-        <v>55</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3278,8 +3278,8 @@
         <v>259</v>
       </c>
       <c r="F82">
-        <f ca="1">ROUND(RAND()*((C82 * 10)-(C82*5))+ C82*5,0)</f>
-        <v>125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3299,8 +3299,8 @@
         <v>255</v>
       </c>
       <c r="F83">
-        <f ca="1">ROUND(RAND()*((C83 * 10)-(C83*5))+ C83*5,0)</f>
-        <v>59</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
         <v>255</v>
       </c>
       <c r="F84">
-        <f ca="1">ROUND(RAND()*((C84 * 10)-(C84*5))+ C84*5,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>41</v>
       </c>
     </row>
@@ -3341,8 +3341,8 @@
         <v>295</v>
       </c>
       <c r="F85">
-        <f ca="1">ROUND(RAND()*((C85 * 10)-(C85*5))+ C85*5,0)</f>
-        <v>44</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,8 +3362,8 @@
         <v>255</v>
       </c>
       <c r="F86">
-        <f ca="1">ROUND(RAND()*((C86 * 10)-(C86*5))+ C86*5,0)</f>
-        <v>82</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,8 +3383,8 @@
         <v>254</v>
       </c>
       <c r="F87">
-        <f ca="1">ROUND(RAND()*((C87 * 10)-(C87*5))+ C87*5,0)</f>
-        <v>48</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3404,8 +3404,8 @@
         <v>256</v>
       </c>
       <c r="F88">
-        <f ca="1">ROUND(RAND()*((C88 * 10)-(C88*5))+ C88*5,0)</f>
-        <v>87</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3425,8 +3425,8 @@
         <v>295</v>
       </c>
       <c r="F89">
-        <f ca="1">ROUND(RAND()*((C89 * 10)-(C89*5))+ C89*5,0)</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3446,8 +3446,8 @@
         <v>295</v>
       </c>
       <c r="F90">
-        <f ca="1">ROUND(RAND()*((C90 * 10)-(C90*5))+ C90*5,0)</f>
-        <v>100</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3467,8 +3467,8 @@
         <v>295</v>
       </c>
       <c r="F91">
-        <f ca="1">ROUND(RAND()*((C91 * 10)-(C91*5))+ C91*5,0)</f>
-        <v>178</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3488,8 +3488,8 @@
         <v>295</v>
       </c>
       <c r="F92">
-        <f ca="1">ROUND(RAND()*((C92 * 10)-(C92*5))+ C92*5,0)</f>
-        <v>70</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3509,8 +3509,8 @@
         <v>295</v>
       </c>
       <c r="F93">
-        <f ca="1">ROUND(RAND()*((C93 * 10)-(C93*5))+ C93*5,0)</f>
-        <v>51</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3530,8 +3530,8 @@
         <v>295</v>
       </c>
       <c r="F94">
-        <f ca="1">ROUND(RAND()*((C94 * 10)-(C94*5))+ C94*5,0)</f>
-        <v>55</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3551,8 +3551,8 @@
         <v>254</v>
       </c>
       <c r="F95">
-        <f ca="1">ROUND(RAND()*((C95 * 10)-(C95*5))+ C95*5,0)</f>
-        <v>97</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3572,8 +3572,8 @@
         <v>245</v>
       </c>
       <c r="F96">
-        <f ca="1">ROUND(RAND()*((C96 * 10)-(C96*5))+ C96*5,0)</f>
-        <v>90</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3593,8 +3593,8 @@
         <v>243</v>
       </c>
       <c r="F97">
-        <f ca="1">ROUND(RAND()*((C97 * 10)-(C97*5))+ C97*5,0)</f>
-        <v>99</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3614,8 +3614,8 @@
         <v>243</v>
       </c>
       <c r="F98">
-        <f ca="1">ROUND(RAND()*((C98 * 10)-(C98*5))+ C98*5,0)</f>
-        <v>51</v>
+        <f t="shared" ref="F98:F129" ca="1" si="3">ROUND(RAND()*((C98 * 10)-(C98*5))+ C98*5,0)</f>
+        <v>35</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3635,8 +3635,8 @@
         <v>243</v>
       </c>
       <c r="F99">
-        <f ca="1">ROUND(RAND()*((C99 * 10)-(C99*5))+ C99*5,0)</f>
-        <v>16</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3656,8 +3656,8 @@
         <v>243</v>
       </c>
       <c r="F100">
-        <f ca="1">ROUND(RAND()*((C100 * 10)-(C100*5))+ C100*5,0)</f>
-        <v>34</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3677,8 +3677,8 @@
         <v>243</v>
       </c>
       <c r="F101">
-        <f ca="1">ROUND(RAND()*((C101 * 10)-(C101*5))+ C101*5,0)</f>
-        <v>52</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3698,8 +3698,8 @@
         <v>243</v>
       </c>
       <c r="F102">
-        <f ca="1">ROUND(RAND()*((C102 * 10)-(C102*5))+ C102*5,0)</f>
-        <v>100</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3719,8 +3719,8 @@
         <v>243</v>
       </c>
       <c r="F103">
-        <f ca="1">ROUND(RAND()*((C103 * 10)-(C103*5))+ C103*5,0)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>124</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3740,8 +3740,8 @@
         <v>243</v>
       </c>
       <c r="F104">
-        <f ca="1">ROUND(RAND()*((C104 * 10)-(C104*5))+ C104*5,0)</f>
-        <v>42</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>36</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3761,8 +3761,8 @@
         <v>242</v>
       </c>
       <c r="F105">
-        <f ca="1">ROUND(RAND()*((C105 * 10)-(C105*5))+ C105*5,0)</f>
-        <v>106</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3782,8 +3782,8 @@
         <v>242</v>
       </c>
       <c r="F106">
-        <f ca="1">ROUND(RAND()*((C106 * 10)-(C106*5))+ C106*5,0)</f>
-        <v>87</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3803,8 +3803,8 @@
         <v>242</v>
       </c>
       <c r="F107">
-        <f ca="1">ROUND(RAND()*((C107 * 10)-(C107*5))+ C107*5,0)</f>
-        <v>65</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>50</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3824,8 +3824,8 @@
         <v>242</v>
       </c>
       <c r="F108">
-        <f ca="1">ROUND(RAND()*((C108 * 10)-(C108*5))+ C108*5,0)</f>
-        <v>59</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3845,8 +3845,8 @@
         <v>242</v>
       </c>
       <c r="F109">
-        <f ca="1">ROUND(RAND()*((C109 * 10)-(C109*5))+ C109*5,0)</f>
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3866,8 +3866,8 @@
         <v>250</v>
       </c>
       <c r="F110">
-        <f ca="1">ROUND(RAND()*((C110 * 10)-(C110*5))+ C110*5,0)</f>
-        <v>51</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3887,8 +3887,8 @@
         <v>250</v>
       </c>
       <c r="F111">
-        <f ca="1">ROUND(RAND()*((C111 * 10)-(C111*5))+ C111*5,0)</f>
-        <v>91</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3908,8 +3908,8 @@
         <v>250</v>
       </c>
       <c r="F112">
-        <f ca="1">ROUND(RAND()*((C112 * 10)-(C112*5))+ C112*5,0)</f>
-        <v>164</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3929,8 +3929,8 @@
         <v>250</v>
       </c>
       <c r="F113">
-        <f ca="1">ROUND(RAND()*((C113 * 10)-(C113*5))+ C113*5,0)</f>
-        <v>96</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3950,8 +3950,8 @@
         <v>243</v>
       </c>
       <c r="F114">
-        <f ca="1">ROUND(RAND()*((C114 * 10)-(C114*5))+ C114*5,0)</f>
-        <v>31</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,8 +3971,8 @@
         <v>246</v>
       </c>
       <c r="F115">
-        <f ca="1">ROUND(RAND()*((C115 * 10)-(C115*5))+ C115*5,0)</f>
-        <v>27</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>25</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3992,8 +3992,8 @@
         <v>243</v>
       </c>
       <c r="F116">
-        <f ca="1">ROUND(RAND()*((C116 * 10)-(C116*5))+ C116*5,0)</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -4013,8 +4013,8 @@
         <v>253</v>
       </c>
       <c r="F117">
-        <f ca="1">ROUND(RAND()*((C117 * 10)-(C117*5))+ C117*5,0)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>31</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -4034,8 +4034,8 @@
         <v>241</v>
       </c>
       <c r="F118">
-        <f ca="1">ROUND(RAND()*((C118 * 10)-(C118*5))+ C118*5,0)</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -4055,8 +4055,8 @@
         <v>241</v>
       </c>
       <c r="F119">
-        <f ca="1">ROUND(RAND()*((C119 * 10)-(C119*5))+ C119*5,0)</f>
-        <v>31</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -4076,8 +4076,8 @@
         <v>241</v>
       </c>
       <c r="F120">
-        <f ca="1">ROUND(RAND()*((C120 * 10)-(C120*5))+ C120*5,0)</f>
-        <v>62</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,8 +4097,8 @@
         <v>241</v>
       </c>
       <c r="F121">
-        <f ca="1">ROUND(RAND()*((C121 * 10)-(C121*5))+ C121*5,0)</f>
-        <v>95</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -4118,8 +4118,8 @@
         <v>241</v>
       </c>
       <c r="F122">
-        <f ca="1">ROUND(RAND()*((C122 * 10)-(C122*5))+ C122*5,0)</f>
-        <v>79</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>53</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -4139,8 +4139,8 @@
         <v>241</v>
       </c>
       <c r="F123">
-        <f ca="1">ROUND(RAND()*((C123 * 10)-(C123*5))+ C123*5,0)</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -4160,8 +4160,8 @@
         <v>241</v>
       </c>
       <c r="F124">
-        <f ca="1">ROUND(RAND()*((C124 * 10)-(C124*5))+ C124*5,0)</f>
-        <v>110</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>106</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -4181,8 +4181,8 @@
         <v>241</v>
       </c>
       <c r="F125">
-        <f ca="1">ROUND(RAND()*((C125 * 10)-(C125*5))+ C125*5,0)</f>
-        <v>117</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>84</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -4202,8 +4202,8 @@
         <v>241</v>
       </c>
       <c r="F126">
-        <f ca="1">ROUND(RAND()*((C126 * 10)-(C126*5))+ C126*5,0)</f>
-        <v>28</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -4223,8 +4223,8 @@
         <v>258</v>
       </c>
       <c r="F127">
-        <f ca="1">ROUND(RAND()*((C127 * 10)-(C127*5))+ C127*5,0)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>59</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -4244,8 +4244,8 @@
         <v>258</v>
       </c>
       <c r="F128">
-        <f ca="1">ROUND(RAND()*((C128 * 10)-(C128*5))+ C128*5,0)</f>
-        <v>116</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>109</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -4265,8 +4265,8 @@
         <v>243</v>
       </c>
       <c r="F129">
-        <f ca="1">ROUND(RAND()*((C129 * 10)-(C129*5))+ C129*5,0)</f>
-        <v>97</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>84</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -4286,8 +4286,8 @@
         <v>243</v>
       </c>
       <c r="F130">
-        <f ca="1">ROUND(RAND()*((C130 * 10)-(C130*5))+ C130*5,0)</f>
-        <v>54</v>
+        <f t="shared" ref="F130:F145" ca="1" si="4">ROUND(RAND()*((C130 * 10)-(C130*5))+ C130*5,0)</f>
+        <v>58</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -4307,8 +4307,8 @@
         <v>242</v>
       </c>
       <c r="F131">
-        <f ca="1">ROUND(RAND()*((C131 * 10)-(C131*5))+ C131*5,0)</f>
-        <v>144</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -4328,8 +4328,8 @@
         <v>250</v>
       </c>
       <c r="F132">
-        <f ca="1">ROUND(RAND()*((C132 * 10)-(C132*5))+ C132*5,0)</f>
-        <v>105</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>75</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -4349,8 +4349,8 @@
         <v>241</v>
       </c>
       <c r="F133">
-        <f ca="1">ROUND(RAND()*((C133 * 10)-(C133*5))+ C133*5,0)</f>
-        <v>82</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -4370,8 +4370,8 @@
         <v>260</v>
       </c>
       <c r="F134">
-        <f ca="1">ROUND(RAND()*((C134 * 10)-(C134*5))+ C134*5,0)</f>
-        <v>59</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>77</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -4391,8 +4391,8 @@
         <v>260</v>
       </c>
       <c r="F135">
-        <f ca="1">ROUND(RAND()*((C135 * 10)-(C135*5))+ C135*5,0)</f>
-        <v>19</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -4412,8 +4412,8 @@
         <v>260</v>
       </c>
       <c r="F136">
-        <f ca="1">ROUND(RAND()*((C136 * 10)-(C136*5))+ C136*5,0)</f>
-        <v>69</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -4433,8 +4433,8 @@
         <v>260</v>
       </c>
       <c r="F137">
-        <f ca="1">ROUND(RAND()*((C137 * 10)-(C137*5))+ C137*5,0)</f>
-        <v>77</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>98</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -4454,8 +4454,8 @@
         <v>260</v>
       </c>
       <c r="F138">
-        <f ca="1">ROUND(RAND()*((C138 * 10)-(C138*5))+ C138*5,0)</f>
-        <v>82</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -4475,8 +4475,8 @@
         <v>260</v>
       </c>
       <c r="F139">
-        <f ca="1">ROUND(RAND()*((C139 * 10)-(C139*5))+ C139*5,0)</f>
-        <v>128</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>168</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -4496,8 +4496,8 @@
         <v>256</v>
       </c>
       <c r="F140">
-        <f ca="1">ROUND(RAND()*((C140 * 10)-(C140*5))+ C140*5,0)</f>
-        <v>104</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>95</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -4517,8 +4517,8 @@
         <v>260</v>
       </c>
       <c r="F141">
-        <f ca="1">ROUND(RAND()*((C141 * 10)-(C141*5))+ C141*5,0)</f>
-        <v>102</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>135</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -4538,8 +4538,8 @@
         <v>260</v>
       </c>
       <c r="F142">
-        <f ca="1">ROUND(RAND()*((C142 * 10)-(C142*5))+ C142*5,0)</f>
-        <v>40</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>37</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -4559,8 +4559,8 @@
         <v>260</v>
       </c>
       <c r="F143">
-        <f ca="1">ROUND(RAND()*((C143 * 10)-(C143*5))+ C143*5,0)</f>
-        <v>57</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>42</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
         <v>246</v>
       </c>
       <c r="F144">
-        <f ca="1">ROUND(RAND()*((C144 * 10)-(C144*5))+ C144*5,0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -4601,8 +4601,8 @@
         <v>260</v>
       </c>
       <c r="F145">
-        <f ca="1">ROUND(RAND()*((C145 * 10)-(C145*5))+ C145*5,0)</f>
-        <v>9</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -4955,9 +4955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93DAFA4D-9B3B-49F6-8E75-439CF17278B6}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="300" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="300" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5000,178 +5000,178 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>261</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E3" t="s">
         <v>263</v>
       </c>
       <c r="F3">
-        <v>900</v>
+        <v>1800</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D4">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F4">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D5">
-        <v>450</v>
+        <v>1200</v>
       </c>
       <c r="E5" t="s">
         <v>264</v>
       </c>
       <c r="F5">
-        <v>3200</v>
+        <v>4300</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D6">
-        <v>2000</v>
+        <v>770</v>
       </c>
       <c r="E6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F6">
-        <v>6200</v>
+        <v>3900</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>238</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F7">
-        <v>-200</v>
+        <v>2200</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D8">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>261</v>
       </c>
       <c r="F8">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -5182,614 +5182,614 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D9">
-        <v>450</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F9">
-        <v>3500</v>
+        <v>100</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D10">
-        <v>550</v>
+        <v>800</v>
       </c>
       <c r="E10" t="s">
         <v>264</v>
       </c>
       <c r="F10">
-        <v>3800</v>
+        <v>3500</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D11">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F11">
-        <v>6800</v>
+        <v>3400</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D12">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="E12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F12">
-        <v>3600</v>
+        <v>6000</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>238</v>
       </c>
       <c r="D13">
-        <v>300</v>
+        <v>4900</v>
       </c>
       <c r="E13" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F13">
-        <v>1800</v>
+        <v>7500</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F14">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E15" t="s">
         <v>263</v>
       </c>
       <c r="F15">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="E16" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D17">
-        <v>80</v>
+        <v>450</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F17">
-        <v>600</v>
+        <v>3200</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D18">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="E18" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F18">
-        <v>4200</v>
+        <v>6200</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="E19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F19">
-        <v>4800</v>
+        <v>1200</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>238</v>
+        <v>55</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="D20">
-        <v>1200</v>
+        <v>400</v>
       </c>
       <c r="E20" t="s">
         <v>264</v>
       </c>
       <c r="F20">
-        <v>4300</v>
+        <v>3100</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>237</v>
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="D21">
-        <v>75</v>
+        <v>2200</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F21">
-        <v>1900</v>
+        <v>7000</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>237</v>
+        <v>57</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="D22">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>238</v>
+        <v>58</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="D23">
-        <v>770</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
         <v>264</v>
       </c>
       <c r="F23">
-        <v>3900</v>
+        <v>2800</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>238</v>
+        <v>59</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="D24">
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="E24" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F24">
-        <v>2200</v>
+        <v>2700</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>236</v>
       </c>
       <c r="D25">
-        <v>200</v>
+        <v>3500</v>
       </c>
       <c r="E25" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F25">
-        <v>1200</v>
+        <v>9200</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>236</v>
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>237</v>
       </c>
       <c r="D26">
-        <v>400</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F26">
-        <v>3100</v>
+        <v>-100</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>236</v>
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>237</v>
       </c>
       <c r="D27">
-        <v>2200</v>
+        <v>450</v>
       </c>
       <c r="E27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F27">
-        <v>7000</v>
+        <v>3500</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>236</v>
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>237</v>
       </c>
       <c r="D28">
-        <v>150</v>
+        <v>550</v>
       </c>
       <c r="E28" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F28">
-        <v>1000</v>
+        <v>3800</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>236</v>
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>237</v>
       </c>
       <c r="D29">
-        <v>200</v>
+        <v>1800</v>
       </c>
       <c r="E29" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F29">
-        <v>2800</v>
+        <v>6800</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>236</v>
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>237</v>
       </c>
       <c r="D30">
-        <v>250</v>
+        <v>900</v>
       </c>
       <c r="E30" t="s">
         <v>264</v>
       </c>
       <c r="F30">
-        <v>2700</v>
+        <v>3600</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>286</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>236</v>
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>237</v>
       </c>
       <c r="D31">
-        <v>3500</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F31">
-        <v>9200</v>
+        <v>800</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D32">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
         <v>261</v>
@@ -5806,39 +5806,39 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D33">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F33">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D34">
         <v>800</v>
@@ -5847,24 +5847,24 @@
         <v>264</v>
       </c>
       <c r="F34">
-        <v>3500</v>
+        <v>4200</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D35">
         <v>1000</v>
@@ -5873,70 +5873,70 @@
         <v>264</v>
       </c>
       <c r="F35">
-        <v>3400</v>
+        <v>4800</v>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D36">
-        <v>3000</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F36">
-        <v>6000</v>
+        <v>1900</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D37">
-        <v>4900</v>
+        <v>60</v>
       </c>
       <c r="E37" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F37">
-        <v>7500</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
-    <sortCondition ref="A1:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
+    <sortCondition ref="C1:C37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5960,7 +5960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC90BD89-F4C0-4E65-AD56-5996B44BD413}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>

</xml_diff>

<commit_message>
created global audio manager
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed100b9df88b388/Documents/GitHub/Fishing-Pomodoro-Timer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="466" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98F0484B-6D7C-4BE6-85FD-A6713C72578D}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF5E3F9-CC94-4069-A8D8-6A1B068612A8}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-1350" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
+    <workbookView minimized="1" xWindow="-19200" yWindow="-1240" windowWidth="19380" windowHeight="11180" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
   </bookViews>
   <sheets>
     <sheet name="catchables" sheetId="1" r:id="rId1"/>
@@ -1548,9 +1548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6B662D-2C96-4B0E-A4D6-1760D360EC42}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="350" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="350" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="H163" sqref="H162:H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F33" ca="1" si="0">ROUND(RAND()*((C2 * 10)-(C2*5))+ C2*5,0)</f>
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>139</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>108</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>118</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="F34">
         <f t="shared" ref="F34:F65" ca="1" si="1">ROUND(RAND()*((C34 * 10)-(C34*5))+ C34*5,0)</f>
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
-        <v>116</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,7 +2523,7 @@
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="1"/>
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="1"/>
-        <v>158</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="F66">
         <f t="shared" ref="F66:F97" ca="1" si="2">ROUND(RAND()*((C66 * 10)-(C66*5))+ C66*5,0)</f>
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="2"/>
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,7 +3069,7 @@
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="2"/>
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="2"/>
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="2"/>
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="2"/>
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="2"/>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="2"/>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="2"/>
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,7 +3426,7 @@
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="2"/>
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="2"/>
-        <v>106</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="2"/>
-        <v>102</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="2"/>
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="2"/>
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="2"/>
-        <v>98</v>
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="2"/>
-        <v>142</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3615,7 +3615,7 @@
       </c>
       <c r="F98">
         <f t="shared" ref="F98:F129" ca="1" si="3">ROUND(RAND()*((C98 * 10)-(C98*5))+ C98*5,0)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3699,7 +3699,7 @@
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="3"/>
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="3"/>
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,7 +3762,7 @@
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="3"/>
-        <v>179</v>
+        <v>133</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="3"/>
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="3"/>
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="3"/>
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="3"/>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3972,7 +3972,7 @@
       </c>
       <c r="F115">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="F116">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="F117">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -4035,7 +4035,7 @@
       </c>
       <c r="F118">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="F119">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="F120">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="F121">
         <f t="shared" ca="1" si="3"/>
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -4119,7 +4119,7 @@
       </c>
       <c r="F122">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -4140,7 +4140,7 @@
       </c>
       <c r="F123">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="F124">
         <f t="shared" ca="1" si="3"/>
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="F125">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="F126">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="F127">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="F128">
         <f t="shared" ca="1" si="3"/>
-        <v>109</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
       </c>
       <c r="F129">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -4287,7 +4287,7 @@
       </c>
       <c r="F130">
         <f t="shared" ref="F130:F145" ca="1" si="4">ROUND(RAND()*((C130 * 10)-(C130*5))+ C130*5,0)</f>
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="F131">
         <f t="shared" ca="1" si="4"/>
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="F132">
         <f t="shared" ca="1" si="4"/>
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="F133">
         <f t="shared" ca="1" si="4"/>
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
       </c>
       <c r="F134">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="F135">
         <f t="shared" ca="1" si="4"/>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="F136">
         <f t="shared" ca="1" si="4"/>
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="F137">
         <f t="shared" ca="1" si="4"/>
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="F138">
         <f t="shared" ca="1" si="4"/>
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="F139">
         <f t="shared" ca="1" si="4"/>
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="F140">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="F141">
         <f t="shared" ca="1" si="4"/>
-        <v>135</v>
+        <v>83</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -4539,7 +4539,7 @@
       </c>
       <c r="F142">
         <f t="shared" ca="1" si="4"/>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="F143">
         <f t="shared" ca="1" si="4"/>
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="F144">
         <f t="shared" ca="1" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="F145">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -4940,6 +4940,9 @@
       </c>
       <c r="E167" t="s">
         <v>248</v>
+      </c>
+      <c r="F167">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -4955,7 +4958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93DAFA4D-9B3B-49F6-8E75-439CF17278B6}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="300" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="300" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>

</xml_diff>

<commit_message>
added icons, refactored json loading, and creating new saves
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed100b9df88b388/Documents/GitHub/Fishing-Pomodoro-Timer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="467" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF5E3F9-CC94-4069-A8D8-6A1B068612A8}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="8_{035C8AE2-BEE5-45CA-8263-7E32D9533727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A11FBA4-3BC0-47C6-BFDF-C5BDFE550A23}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-19200" yWindow="-1240" windowWidth="19380" windowHeight="11180" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E5EF41F-42D3-4D64-83EA-60F358F1DA3F}"/>
   </bookViews>
   <sheets>
     <sheet name="catchables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="306">
   <si>
     <t>Name</t>
   </si>
@@ -927,6 +927,36 @@
   </si>
   <si>
     <t>Tropical</t>
+  </si>
+  <si>
+    <t>catchable type</t>
+  </si>
+  <si>
+    <t>catchable name</t>
+  </si>
+  <si>
+    <t>Warm Waters Only</t>
+  </si>
+  <si>
+    <t>Catch 10 tropical fish</t>
+  </si>
+  <si>
+    <t>Creeper Sweep</t>
+  </si>
+  <si>
+    <t>Find some creepy crawlies</t>
+  </si>
+  <si>
+    <t>Junk in the Trunk</t>
+  </si>
+  <si>
+    <t>Ok freak</t>
+  </si>
+  <si>
+    <t>Deep Dive</t>
+  </si>
+  <si>
+    <t>Catch 1 deep fish</t>
   </si>
 </sst>
 </file>
@@ -1549,8 +1579,8 @@
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="350" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H163" sqref="H162:H163"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1629,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F33" ca="1" si="0">ROUND(RAND()*((C2 * 10)-(C2*5))+ C2*5,0)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1620,7 +1650,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,7 +1671,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,7 +1692,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1713,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +1734,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,7 +1755,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1746,7 +1776,7 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,7 +1797,7 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1788,7 +1818,7 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1809,7 +1839,7 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,7 +1860,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,7 +1881,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1902,7 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>132</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1893,7 +1923,7 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>143</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,7 +1944,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1935,7 +1965,7 @@
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,7 +1986,7 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,7 +2007,7 @@
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,7 +2028,7 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2049,7 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,7 +2070,7 @@
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,7 +2091,7 @@
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2082,7 +2112,7 @@
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2103,7 +2133,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,7 +2154,7 @@
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2145,7 +2175,7 @@
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2166,7 +2196,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,7 +2217,7 @@
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,7 +2238,7 @@
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,7 +2259,7 @@
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,7 +2280,7 @@
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,7 +2301,7 @@
       </c>
       <c r="F34">
         <f t="shared" ref="F34:F65" ca="1" si="1">ROUND(RAND()*((C34 * 10)-(C34*5))+ C34*5,0)</f>
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,7 +2322,7 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,7 +2343,7 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,7 +2364,7 @@
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,7 +2385,7 @@
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,7 +2406,7 @@
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,7 +2427,7 @@
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
-        <v>177</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,7 +2448,7 @@
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,7 +2469,7 @@
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,7 +2490,7 @@
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2511,7 @@
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="1"/>
-        <v>109</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,7 +2532,7 @@
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,7 +2553,7 @@
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,7 +2574,7 @@
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,7 +2595,7 @@
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,7 +2616,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,7 +2637,7 @@
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,7 +2658,7 @@
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,7 +2679,7 @@
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="1"/>
-        <v>148</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,7 +2700,7 @@
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,7 +2721,7 @@
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,7 +2742,7 @@
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,7 +2763,7 @@
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2754,7 +2784,7 @@
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,7 +2805,7 @@
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,7 +2826,7 @@
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2817,7 +2847,7 @@
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2838,7 +2868,7 @@
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="1"/>
-        <v>119</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2859,7 +2889,7 @@
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2880,7 +2910,7 @@
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,7 +2931,7 @@
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="1"/>
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,7 +2952,7 @@
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="1"/>
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2943,7 +2973,7 @@
       </c>
       <c r="F66">
         <f t="shared" ref="F66:F97" ca="1" si="2">ROUND(RAND()*((C66 * 10)-(C66*5))+ C66*5,0)</f>
-        <v>76</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,7 +2994,7 @@
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,7 +3015,7 @@
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="2"/>
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3006,7 +3036,7 @@
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3027,7 +3057,7 @@
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,7 +3078,7 @@
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="2"/>
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,7 +3099,7 @@
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="2"/>
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3090,7 +3120,7 @@
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="2"/>
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3107,11 +3137,11 @@
         <v>150</v>
       </c>
       <c r="E74" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,7 +3204,7 @@
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3191,11 +3221,11 @@
         <v>800</v>
       </c>
       <c r="E78" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3216,7 +3246,7 @@
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,7 +3267,7 @@
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3258,7 +3288,7 @@
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="2"/>
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -3279,7 +3309,7 @@
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,7 +3330,7 @@
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3342,7 +3372,7 @@
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="2"/>
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3363,7 +3393,7 @@
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="2"/>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3384,7 +3414,7 @@
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3405,7 +3435,7 @@
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="2"/>
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -3422,11 +3452,11 @@
         <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="2"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3443,11 +3473,11 @@
         <v>14</v>
       </c>
       <c r="E90" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,11 +3494,11 @@
         <v>9</v>
       </c>
       <c r="E91" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="2"/>
-        <v>176</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3485,11 +3515,11 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3506,11 +3536,11 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="2"/>
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3527,11 +3557,11 @@
         <v>3</v>
       </c>
       <c r="E94" t="s">
-        <v>295</v>
+        <v>240</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="2"/>
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3552,7 +3582,7 @@
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3573,7 +3603,7 @@
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="2"/>
-        <v>53</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,7 +3624,7 @@
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="2"/>
-        <v>106</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3615,7 +3645,7 @@
       </c>
       <c r="F98">
         <f t="shared" ref="F98:F129" ca="1" si="3">ROUND(RAND()*((C98 * 10)-(C98*5))+ C98*5,0)</f>
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3636,7 +3666,7 @@
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,7 +3687,7 @@
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,7 +3708,7 @@
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3699,7 +3729,7 @@
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="3"/>
-        <v>115</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3720,7 +3750,7 @@
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="3"/>
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3741,7 +3771,7 @@
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3783,7 +3813,7 @@
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="3"/>
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3804,7 +3834,7 @@
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="3"/>
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3846,7 +3876,7 @@
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3867,7 +3897,7 @@
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="3"/>
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3888,7 +3918,7 @@
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="3"/>
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -3909,7 +3939,7 @@
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="3"/>
-        <v>96</v>
+        <v>158</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3930,7 +3960,7 @@
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3951,7 +3981,7 @@
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3972,7 +4002,7 @@
       </c>
       <c r="F115">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3993,7 +4023,7 @@
       </c>
       <c r="F116">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -4014,7 +4044,7 @@
       </c>
       <c r="F117">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -4035,7 +4065,7 @@
       </c>
       <c r="F118">
         <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -4056,7 +4086,7 @@
       </c>
       <c r="F119">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -4077,7 +4107,7 @@
       </c>
       <c r="F120">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -4098,7 +4128,7 @@
       </c>
       <c r="F121">
         <f t="shared" ca="1" si="3"/>
-        <v>132</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -4119,7 +4149,7 @@
       </c>
       <c r="F122">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -4140,7 +4170,7 @@
       </c>
       <c r="F123">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,7 +4191,7 @@
       </c>
       <c r="F124">
         <f t="shared" ca="1" si="3"/>
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -4182,7 +4212,7 @@
       </c>
       <c r="F125">
         <f t="shared" ca="1" si="3"/>
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -4203,7 +4233,7 @@
       </c>
       <c r="F126">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -4224,7 +4254,7 @@
       </c>
       <c r="F127">
         <f t="shared" ca="1" si="3"/>
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -4245,7 +4275,7 @@
       </c>
       <c r="F128">
         <f t="shared" ca="1" si="3"/>
-        <v>189</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -4266,7 +4296,7 @@
       </c>
       <c r="F129">
         <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -4287,7 +4317,7 @@
       </c>
       <c r="F130">
         <f t="shared" ref="F130:F145" ca="1" si="4">ROUND(RAND()*((C130 * 10)-(C130*5))+ C130*5,0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -4308,7 +4338,7 @@
       </c>
       <c r="F131">
         <f t="shared" ca="1" si="4"/>
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -4329,7 +4359,7 @@
       </c>
       <c r="F132">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -4350,7 +4380,7 @@
       </c>
       <c r="F133">
         <f t="shared" ca="1" si="4"/>
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,7 +4401,7 @@
       </c>
       <c r="F134">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -4392,7 +4422,7 @@
       </c>
       <c r="F135">
         <f t="shared" ca="1" si="4"/>
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -4413,7 +4443,7 @@
       </c>
       <c r="F136">
         <f t="shared" ca="1" si="4"/>
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -4434,7 +4464,7 @@
       </c>
       <c r="F137">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -4455,7 +4485,7 @@
       </c>
       <c r="F138">
         <f t="shared" ca="1" si="4"/>
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -4476,7 +4506,7 @@
       </c>
       <c r="F139">
         <f t="shared" ca="1" si="4"/>
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -4497,7 +4527,7 @@
       </c>
       <c r="F140">
         <f t="shared" ca="1" si="4"/>
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -4518,7 +4548,7 @@
       </c>
       <c r="F141">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -4539,7 +4569,7 @@
       </c>
       <c r="F142">
         <f t="shared" ca="1" si="4"/>
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -4560,7 +4590,7 @@
       </c>
       <c r="F143">
         <f t="shared" ca="1" si="4"/>
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,7 +4611,7 @@
       </c>
       <c r="F144">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -4602,7 +4632,7 @@
       </c>
       <c r="F145">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -4960,7 +4990,7 @@
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="300" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,178 +5033,178 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>261</v>
       </c>
       <c r="F2">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D3">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
         <v>263</v>
       </c>
       <c r="F3">
-        <v>1800</v>
+        <v>900</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F4">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D5">
-        <v>1200</v>
+        <v>450</v>
       </c>
       <c r="E5" t="s">
         <v>264</v>
       </c>
       <c r="F5">
-        <v>4300</v>
+        <v>3200</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D6">
-        <v>770</v>
+        <v>2000</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F6">
-        <v>3900</v>
+        <v>6200</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>238</v>
       </c>
       <c r="D7">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F7">
-        <v>2200</v>
+        <v>-200</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>261</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -5185,614 +5215,614 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>450</v>
       </c>
       <c r="E9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>3500</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D10">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="E10" t="s">
         <v>264</v>
       </c>
       <c r="F10">
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D11">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="E11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F11">
-        <v>3400</v>
+        <v>6800</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D12">
-        <v>3000</v>
+        <v>900</v>
       </c>
       <c r="E12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F12">
-        <v>6000</v>
+        <v>3600</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>238</v>
       </c>
       <c r="D13">
-        <v>4900</v>
+        <v>300</v>
       </c>
       <c r="E13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F13">
-        <v>7500</v>
+        <v>1800</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14">
+        <v>2500</v>
+      </c>
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>236</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>261</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D15">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
         <v>263</v>
       </c>
       <c r="F15">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D16">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F16">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D17">
-        <v>450</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F17">
-        <v>3200</v>
+        <v>600</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D18">
-        <v>2000</v>
+        <v>800</v>
       </c>
       <c r="E18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F18">
-        <v>6200</v>
+        <v>4200</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D19">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="E19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F19">
-        <v>1200</v>
+        <v>4800</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>236</v>
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>238</v>
       </c>
       <c r="D20">
-        <v>400</v>
+        <v>1200</v>
       </c>
       <c r="E20" t="s">
         <v>264</v>
       </c>
       <c r="F20">
-        <v>3100</v>
+        <v>4300</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>236</v>
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>237</v>
       </c>
       <c r="D21">
-        <v>2200</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F21">
-        <v>7000</v>
+        <v>1900</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>236</v>
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
       </c>
       <c r="D22">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F22">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>236</v>
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>238</v>
       </c>
       <c r="D23">
-        <v>200</v>
+        <v>770</v>
       </c>
       <c r="E23" t="s">
         <v>264</v>
       </c>
       <c r="F23">
-        <v>2800</v>
+        <v>3900</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>238</v>
+      </c>
+      <c r="D24">
+        <v>120</v>
+      </c>
+      <c r="E24" t="s">
+        <v>263</v>
+      </c>
+      <c r="F24">
+        <v>2200</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25" t="s">
+        <v>263</v>
+      </c>
+      <c r="F25">
+        <v>1200</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26">
+        <v>400</v>
+      </c>
+      <c r="E26" t="s">
+        <v>264</v>
+      </c>
+      <c r="F26">
+        <v>3100</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27">
+        <v>2200</v>
+      </c>
+      <c r="E27" t="s">
+        <v>265</v>
+      </c>
+      <c r="F27">
+        <v>7000</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28">
+        <v>150</v>
+      </c>
+      <c r="E28" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29">
+        <v>200</v>
+      </c>
+      <c r="E29" t="s">
+        <v>264</v>
+      </c>
+      <c r="F29">
+        <v>2800</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D24">
+      <c r="D30">
         <v>250</v>
-      </c>
-      <c r="E24" t="s">
-        <v>264</v>
-      </c>
-      <c r="F24">
-        <v>2700</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D25">
-        <v>3500</v>
-      </c>
-      <c r="E25" t="s">
-        <v>266</v>
-      </c>
-      <c r="F25">
-        <v>9200</v>
-      </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>237</v>
-      </c>
-      <c r="D26">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>261</v>
-      </c>
-      <c r="F26">
-        <v>-100</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27">
-        <v>450</v>
-      </c>
-      <c r="E27" t="s">
-        <v>264</v>
-      </c>
-      <c r="F27">
-        <v>3500</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>9</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>237</v>
-      </c>
-      <c r="D28">
-        <v>550</v>
-      </c>
-      <c r="E28" t="s">
-        <v>264</v>
-      </c>
-      <c r="F28">
-        <v>3800</v>
-      </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>237</v>
-      </c>
-      <c r="D29">
-        <v>1800</v>
-      </c>
-      <c r="E29" t="s">
-        <v>265</v>
-      </c>
-      <c r="F29">
-        <v>6800</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
-      </c>
-      <c r="H29" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>11</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" t="s">
-        <v>237</v>
-      </c>
-      <c r="D30">
-        <v>900</v>
       </c>
       <c r="E30" t="s">
         <v>264</v>
       </c>
       <c r="F30">
-        <v>3600</v>
+        <v>2700</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" t="s">
-        <v>237</v>
+        <v>60</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>3500</v>
       </c>
       <c r="E31" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F31">
-        <v>800</v>
+        <v>9200</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H31" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D32">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
         <v>261</v>
@@ -5809,39 +5839,39 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D33">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F33">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D34">
         <v>800</v>
@@ -5850,24 +5880,24 @@
         <v>264</v>
       </c>
       <c r="F34">
-        <v>4200</v>
+        <v>3500</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D35">
         <v>1000</v>
@@ -5876,70 +5906,70 @@
         <v>264</v>
       </c>
       <c r="F35">
-        <v>4800</v>
+        <v>3400</v>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D36">
-        <v>75</v>
+        <v>3000</v>
       </c>
       <c r="E36" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F36">
-        <v>1900</v>
+        <v>6000</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D37">
-        <v>60</v>
+        <v>4900</v>
       </c>
       <c r="E37" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
-    <sortCondition ref="C1:C37"/>
+    <sortCondition ref="A1:A37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5961,27 +5991,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC90BD89-F4C0-4E65-AD56-5996B44BD413}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6004,10 +6035,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="I1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6018,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -6027,7 +6061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6038,7 +6072,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>2000</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
@@ -6050,7 +6084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -6061,7 +6095,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>1500</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -6070,7 +6104,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6081,25 +6115,117 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G5">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{274EC504-EC7C-4561-86A6-41FDC635D659}">
           <x14:formula1>
             <xm:f>Dropdowns!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{354DD619-94E4-4AD3-81CE-C1D790B0E1AD}">
+          <x14:formula1>
+            <xm:f>gear!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F8DD316-D5E7-4D5C-A499-C7FC760C26C3}">
+          <x14:formula1>
+            <xm:f>catchables!$E$2:$E$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>